<commit_message>
Makefile changes: adding time function to make run
</commit_message>
<xml_diff>
--- a/Medições de Tempo.xlsx
+++ b/Medições de Tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasestevao/Documents/Git/Parallel-Programming-OpenMP-Jacobi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF24457-60A6-C24E-BB4B-357885ACC880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B1F020-EF4D-A643-B419-D94B49AEB4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{556A7405-AA75-BF40-8595-E9339ADE3663}"/>
   </bookViews>
@@ -3093,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA73BE4E-7CBC-834B-B2B7-9530EF8EDF7F}">
   <dimension ref="A1:BR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="AY8" sqref="AY8"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="BO2" sqref="BO2:BR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3740,15 +3740,15 @@
       <c r="BJ5" s="13">
         <v>2</v>
       </c>
-      <c r="BK5" s="12">
+      <c r="BK5" s="18">
         <f>AZ9/AZ6</f>
         <v>1.9437585733882035</v>
       </c>
-      <c r="BL5" s="12">
+      <c r="BL5" s="18">
         <f>BC9/BC6</f>
         <v>2.0295741000082375</v>
       </c>
-      <c r="BM5" s="12">
+      <c r="BM5" s="18">
         <f>BF9/BF6</f>
         <v>1.983803064007148</v>
       </c>
@@ -3919,15 +3919,15 @@
       <c r="BJ6" s="13">
         <v>4</v>
       </c>
-      <c r="BK6" s="12">
+      <c r="BK6" s="18">
         <f>AZ9/AZ7</f>
         <v>3.5964467005076171</v>
       </c>
-      <c r="BL6" s="12">
+      <c r="BL6" s="18">
         <f>BC9/BC7</f>
         <v>3.9056753329105893</v>
       </c>
-      <c r="BM6" s="12">
+      <c r="BM6" s="18">
         <f>BF9/BF7</f>
         <v>3.9168229407133559</v>
       </c>
@@ -4098,15 +4098,15 @@
       <c r="BJ7" s="13">
         <v>8</v>
       </c>
-      <c r="BK7" s="12">
+      <c r="BK7" s="18">
         <f>AZ9/AZ8</f>
         <v>5.3776091081593949</v>
       </c>
-      <c r="BL7" s="12">
+      <c r="BL7" s="18">
         <f>BC9/BC8</f>
         <v>6.8076816800221058</v>
       </c>
-      <c r="BM7" s="12">
+      <c r="BM7" s="18">
         <f>BF9/BF8</f>
         <v>6.8882012954777307</v>
       </c>

</xml_diff>